<commit_message>
Crowdfunding ETL and database setup
</commit_message>
<xml_diff>
--- a/crowdfunding.xlsx
+++ b/crowdfunding.xlsx
@@ -1,22 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tberton/Sandbox/M8-ETL/M8-Async/Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/radatus/Desktop/GitHub/Crowdfunding-ETL_Ch8/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D30995-0CA2-CD4A-A0F0-5AA998D31CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECDD015-3020-DE4F-9C22-EA288EBAEFD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="980" windowWidth="28560" windowHeight="14600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="2280" windowWidth="28560" windowHeight="14600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="crowdfunding_info" sheetId="1" r:id="rId1"/>
     <sheet name="contact_info" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -9155,12 +9168,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9499,10 +9511,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9515,7 +9529,7 @@
     <col min="14" max="14" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -53566,10 +53580,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:A1004"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <pane ySplit="4" topLeftCell="A387" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A446" sqref="A446"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>